<commit_message>
Final Front End Commit
</commit_message>
<xml_diff>
--- a/Testing/Front_End/Control.xlsx
+++ b/Testing/Front_End/Control.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\EEVengers\DSO_Testing\Front End\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\EEVengers\Testing\Front_End\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{544117FF-C430-4399-B1B2-182E1A816222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94620B4-B1B9-49BA-BB1C-716758E232F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="3630" windowWidth="28800" windowHeight="11385"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3173,11 +3184,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C499"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AF14" sqref="AF14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>